<commit_message>
Adding Serbian dummy data.
</commit_message>
<xml_diff>
--- a/data/standard_lists/whitelist-dummy.xlsx
+++ b/data/standard_lists/whitelist-dummy.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14340" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14340" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="municipalities" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="210">
   <si>
     <t>albanian</t>
   </si>
@@ -699,8 +699,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -723,7 +737,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -733,6 +747,13 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -742,6 +763,13 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1548,8 +1576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1585,8 +1613,14 @@
       <c r="B2" t="s">
         <v>109</v>
       </c>
+      <c r="C2" t="s">
+        <v>109</v>
+      </c>
       <c r="D2" t="s">
         <v>208</v>
+      </c>
+      <c r="E2" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1596,8 +1630,14 @@
       <c r="B3" t="s">
         <v>110</v>
       </c>
+      <c r="C3" t="s">
+        <v>110</v>
+      </c>
       <c r="D3" t="s">
         <v>158</v>
+      </c>
+      <c r="E3" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1607,8 +1647,14 @@
       <c r="B4" t="s">
         <v>156</v>
       </c>
+      <c r="C4" t="s">
+        <v>156</v>
+      </c>
       <c r="D4" t="s">
         <v>159</v>
+      </c>
+      <c r="E4" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1618,8 +1664,14 @@
       <c r="B5" t="s">
         <v>157</v>
       </c>
+      <c r="C5" t="s">
+        <v>157</v>
+      </c>
       <c r="D5" t="s">
         <v>160</v>
+      </c>
+      <c r="E5" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1629,8 +1681,14 @@
       <c r="B6" t="s">
         <v>116</v>
       </c>
+      <c r="C6" t="s">
+        <v>116</v>
+      </c>
       <c r="D6" t="s">
         <v>161</v>
+      </c>
+      <c r="E6" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1640,8 +1698,14 @@
       <c r="B7" t="s">
         <v>100</v>
       </c>
+      <c r="C7" t="s">
+        <v>100</v>
+      </c>
       <c r="D7" t="s">
         <v>162</v>
+      </c>
+      <c r="E7" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1651,8 +1715,14 @@
       <c r="B8" t="s">
         <v>101</v>
       </c>
+      <c r="C8" t="s">
+        <v>101</v>
+      </c>
       <c r="D8" t="s">
         <v>163</v>
+      </c>
+      <c r="E8" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1662,8 +1732,14 @@
       <c r="B9" t="s">
         <v>102</v>
       </c>
+      <c r="C9" t="s">
+        <v>102</v>
+      </c>
       <c r="D9" t="s">
         <v>164</v>
+      </c>
+      <c r="E9" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1673,8 +1749,14 @@
       <c r="B10" t="s">
         <v>103</v>
       </c>
+      <c r="C10" t="s">
+        <v>103</v>
+      </c>
       <c r="D10" t="s">
         <v>165</v>
+      </c>
+      <c r="E10" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1684,8 +1766,14 @@
       <c r="B11" t="s">
         <v>108</v>
       </c>
+      <c r="C11" t="s">
+        <v>108</v>
+      </c>
       <c r="D11" t="s">
         <v>166</v>
+      </c>
+      <c r="E11" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1695,8 +1783,14 @@
       <c r="B12" t="s">
         <v>117</v>
       </c>
+      <c r="C12" t="s">
+        <v>117</v>
+      </c>
       <c r="D12" t="s">
         <v>167</v>
+      </c>
+      <c r="E12" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1706,8 +1800,14 @@
       <c r="B13" t="s">
         <v>104</v>
       </c>
+      <c r="C13" t="s">
+        <v>104</v>
+      </c>
       <c r="D13" t="s">
         <v>168</v>
+      </c>
+      <c r="E13" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1717,8 +1817,14 @@
       <c r="B14" t="s">
         <v>118</v>
       </c>
+      <c r="C14" t="s">
+        <v>118</v>
+      </c>
       <c r="D14" t="s">
         <v>169</v>
+      </c>
+      <c r="E14" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1728,8 +1834,14 @@
       <c r="B15" t="s">
         <v>106</v>
       </c>
+      <c r="C15" t="s">
+        <v>106</v>
+      </c>
       <c r="D15" t="s">
         <v>170</v>
+      </c>
+      <c r="E15" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1739,228 +1851,354 @@
       <c r="B16" t="s">
         <v>126</v>
       </c>
+      <c r="C16" t="s">
+        <v>126</v>
+      </c>
       <c r="D16" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>107</v>
       </c>
       <c r="B17" t="s">
         <v>107</v>
       </c>
+      <c r="C17" t="s">
+        <v>107</v>
+      </c>
       <c r="D17" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>112</v>
       </c>
       <c r="B18" t="s">
         <v>112</v>
       </c>
+      <c r="C18" t="s">
+        <v>112</v>
+      </c>
       <c r="D18" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>111</v>
       </c>
       <c r="B19" t="s">
         <v>111</v>
       </c>
+      <c r="C19" t="s">
+        <v>111</v>
+      </c>
       <c r="D19" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>113</v>
       </c>
       <c r="B20" t="s">
         <v>113</v>
       </c>
+      <c r="C20" t="s">
+        <v>113</v>
+      </c>
       <c r="D20" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>105</v>
       </c>
       <c r="B21" t="s">
         <v>105</v>
       </c>
+      <c r="C21" t="s">
+        <v>105</v>
+      </c>
       <c r="D21" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>98</v>
       </c>
       <c r="B22" t="s">
         <v>98</v>
       </c>
+      <c r="C22" t="s">
+        <v>98</v>
+      </c>
       <c r="D22" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>114</v>
       </c>
       <c r="B23" t="s">
         <v>114</v>
       </c>
+      <c r="C23" t="s">
+        <v>114</v>
+      </c>
       <c r="D23" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>119</v>
       </c>
       <c r="B24" t="s">
         <v>119</v>
       </c>
+      <c r="C24" t="s">
+        <v>119</v>
+      </c>
       <c r="D24" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>121</v>
       </c>
       <c r="B25" t="s">
         <v>121</v>
       </c>
+      <c r="C25" t="s">
+        <v>121</v>
+      </c>
       <c r="D25" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>122</v>
       </c>
       <c r="B26" t="s">
         <v>122</v>
       </c>
+      <c r="C26" t="s">
+        <v>122</v>
+      </c>
       <c r="D26" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>123</v>
       </c>
       <c r="B27" t="s">
         <v>123</v>
       </c>
+      <c r="C27" t="s">
+        <v>123</v>
+      </c>
       <c r="D27" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>124</v>
       </c>
       <c r="B28" t="s">
         <v>124</v>
       </c>
+      <c r="C28" t="s">
+        <v>124</v>
+      </c>
       <c r="D28" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>125</v>
       </c>
       <c r="B29" t="s">
         <v>125</v>
       </c>
+      <c r="C29" t="s">
+        <v>125</v>
+      </c>
       <c r="D29" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>115</v>
       </c>
       <c r="B30" t="s">
         <v>115</v>
       </c>
+      <c r="C30" t="s">
+        <v>115</v>
+      </c>
       <c r="D30" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E30" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>127</v>
       </c>
       <c r="B31" t="s">
         <v>127</v>
       </c>
+      <c r="C31" t="s">
+        <v>127</v>
+      </c>
       <c r="D31" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="E31" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>120</v>
       </c>
       <c r="B32" t="s">
         <v>120</v>
       </c>
+      <c r="C32" t="s">
+        <v>120</v>
+      </c>
       <c r="D32" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>128</v>
       </c>
       <c r="B33" t="s">
         <v>128</v>
       </c>
+      <c r="C33" t="s">
+        <v>128</v>
+      </c>
       <c r="D33" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="E33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>129</v>
       </c>
       <c r="B34" t="s">
         <v>129</v>
       </c>
+      <c r="C34" t="s">
+        <v>129</v>
+      </c>
       <c r="D34" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="E34" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>130</v>
       </c>
       <c r="B35" t="s">
         <v>130</v>
       </c>
+      <c r="C35" t="s">
+        <v>130</v>
+      </c>
       <c r="D35" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="E35" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>131</v>
       </c>
       <c r="B36" t="s">
         <v>131</v>
       </c>
+      <c r="C36" t="s">
+        <v>131</v>
+      </c>
       <c r="D36" t="s">
         <v>209</v>
+      </c>
+      <c r="E36" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -1978,8 +2216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2014,8 +2252,14 @@
       <c r="B2" t="s">
         <v>194</v>
       </c>
+      <c r="C2" t="s">
+        <v>194</v>
+      </c>
       <c r="D2" t="s">
         <v>207</v>
+      </c>
+      <c r="E2" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2025,8 +2269,14 @@
       <c r="B3" t="s">
         <v>191</v>
       </c>
+      <c r="C3" t="s">
+        <v>191</v>
+      </c>
       <c r="D3" t="s">
         <v>195</v>
+      </c>
+      <c r="E3" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2036,8 +2286,14 @@
       <c r="B4" t="s">
         <v>147</v>
       </c>
+      <c r="C4" t="s">
+        <v>147</v>
+      </c>
       <c r="D4" t="s">
         <v>196</v>
+      </c>
+      <c r="E4" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2047,8 +2303,14 @@
       <c r="B5" t="s">
         <v>145</v>
       </c>
+      <c r="C5" t="s">
+        <v>145</v>
+      </c>
       <c r="D5" t="s">
         <v>197</v>
+      </c>
+      <c r="E5" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2058,8 +2320,14 @@
       <c r="B6" t="s">
         <v>192</v>
       </c>
+      <c r="C6" t="s">
+        <v>192</v>
+      </c>
       <c r="D6" t="s">
         <v>198</v>
+      </c>
+      <c r="E6" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -2069,8 +2337,14 @@
       <c r="B7" t="s">
         <v>148</v>
       </c>
+      <c r="C7" t="s">
+        <v>148</v>
+      </c>
       <c r="D7" t="s">
         <v>199</v>
+      </c>
+      <c r="E7" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -2080,8 +2354,14 @@
       <c r="B8" t="s">
         <v>149</v>
       </c>
+      <c r="C8" t="s">
+        <v>149</v>
+      </c>
       <c r="D8" t="s">
         <v>200</v>
+      </c>
+      <c r="E8" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -2091,8 +2371,14 @@
       <c r="B9" t="s">
         <v>150</v>
       </c>
+      <c r="C9" t="s">
+        <v>150</v>
+      </c>
       <c r="D9" t="s">
         <v>201</v>
+      </c>
+      <c r="E9" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2102,8 +2388,14 @@
       <c r="B10" t="s">
         <v>146</v>
       </c>
+      <c r="C10" t="s">
+        <v>146</v>
+      </c>
       <c r="D10" t="s">
         <v>202</v>
+      </c>
+      <c r="E10" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2113,8 +2405,14 @@
       <c r="B11" t="s">
         <v>151</v>
       </c>
+      <c r="C11" t="s">
+        <v>151</v>
+      </c>
       <c r="D11" t="s">
         <v>203</v>
+      </c>
+      <c r="E11" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -2124,8 +2422,14 @@
       <c r="B12" t="s">
         <v>144</v>
       </c>
+      <c r="C12" t="s">
+        <v>144</v>
+      </c>
       <c r="D12" t="s">
         <v>204</v>
+      </c>
+      <c r="E12" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2135,8 +2439,14 @@
       <c r="B13" t="s">
         <v>193</v>
       </c>
+      <c r="C13" t="s">
+        <v>193</v>
+      </c>
       <c r="D13" t="s">
         <v>206</v>
+      </c>
+      <c r="E13" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -2146,8 +2456,14 @@
       <c r="B14" t="s">
         <v>141</v>
       </c>
+      <c r="C14" t="s">
+        <v>141</v>
+      </c>
       <c r="D14" t="s">
         <v>205</v>
+      </c>
+      <c r="E14" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>